<commit_message>
[PHOENIX-6796] UI : Completed the creation of registration of building approval with flow for a land greater than 10000SQFT
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -265,6 +265,90 @@
   </si>
   <si>
     <t xml:space="preserve">B.Veeraswamy/REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syedBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town Planning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junior Assistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syed/R-Junior Assistant-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rishiBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rishi/R-Assistant-engineer-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sankarBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town Planning Building Overseer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sankar/TPBO-Town Planning Building Overseer-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">satyamBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superintendent of NOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">satyam/NOC-Superintendent-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sathishBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant executive engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sathish/AEE-Assistant executive engineer-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manikantaBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manikanta/EE-Executive engineer-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rishiCorpBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporation Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rishi/CORP-Corporation Engineer-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pradeepBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pradeep/SEC-Secretary-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaibhavBPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superintendent of Approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaibhav/APPVL-Superintendent-01</t>
   </si>
 </sst>
 </file>
@@ -274,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -298,6 +382,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -305,16 +402,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
       <color rgb="FF333333"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -359,7 +449,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,19 +459,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,318 +493,319 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.5918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.5102040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="50.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" s="2" customFormat="true" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -723,49 +814,49 @@
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" s="2" customFormat="true" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -774,73 +865,199 @@
       <c r="D22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -866,6 +1083,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -889,6 +1109,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-5999] Modified the user of assistant engineer
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -99,24 +99,24 @@
     <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
   </si>
   <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
     <t xml:space="preserve">engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer1</t>
-  </si>
-  <si>
     <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
   </si>
   <si>
@@ -213,10 +213,10 @@
     <t xml:space="preserve">Forward to Accounts</t>
   </si>
   <si>
+    <t xml:space="preserve">assis_Engineer_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">assis_Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assis_Engineer_1</t>
   </si>
   <si>
     <t xml:space="preserve">DeputyExecutiveEngineer_1</t>
@@ -495,18 +495,18 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.5102040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="50.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,7 +1063,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1084,12 +1084,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1110,12 +1110,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6796] UI : Updated the user details in New BPA Application Feature and tested the workflow
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -267,88 +267,88 @@
     <t xml:space="preserve">B.Veeraswamy/REV_Revenue Officer_3</t>
   </si>
   <si>
-    <t xml:space="preserve">syedBPA</t>
+    <t xml:space="preserve">ulbOperator</t>
   </si>
   <si>
     <t xml:space="preserve">Town Planning</t>
   </si>
   <si>
-    <t xml:space="preserve">Junior Assistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">syed/R-Junior Assistant-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rishiBPA</t>
+    <t xml:space="preserve">sa1/TP_Senior Assistant_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assistantEngineerBPA</t>
   </si>
   <si>
     <t xml:space="preserve">Assistant engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">rishi/R-Assistant-engineer-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sankarBPA</t>
+    <t xml:space="preserve">AE1/TP_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overseer</t>
   </si>
   <si>
     <t xml:space="preserve">Town Planning Building Overseer</t>
   </si>
   <si>
-    <t xml:space="preserve">sankar/TPBO-Town Planning Building Overseer-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">satyamBPA</t>
+    <t xml:space="preserve">PWO1/TP_Town Planning Building Overseer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">superintendentOfNOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administration</t>
   </si>
   <si>
     <t xml:space="preserve">Superintendent of NOC</t>
   </si>
   <si>
-    <t xml:space="preserve">satyam/NOC-Superintendent-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sathishBPA</t>
+    <t xml:space="preserve">SUPNOC1/ADM_Superintendent of NOC_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assistantExecutiveEngineer</t>
   </si>
   <si>
     <t xml:space="preserve">Assistant executive engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">sathish/AEE-Assistant executive engineer-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manikantaBPA</t>
+    <t xml:space="preserve">AEE1/TP_Assistant Executive Engineer_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">executiveEngineer</t>
   </si>
   <si>
     <t xml:space="preserve">Executive engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">manikanta/EE-Executive engineer-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rishiCorpBPA</t>
+    <t xml:space="preserve">EE1/TP_Executive Engineer_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corporationEngineer</t>
   </si>
   <si>
     <t xml:space="preserve">Corporation Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">rishi/CORP-Corporation Engineer-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pradeepBPA</t>
+    <t xml:space="preserve">CORPENG1/TP_Corporation Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secretary</t>
   </si>
   <si>
     <t xml:space="preserve">Secretary</t>
   </si>
   <si>
-    <t xml:space="preserve">pradeep/SEC-Secretary-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaibhavBPA</t>
+    <t xml:space="preserve">SECRETARY1/ADM_Secretary_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">superintendentOfApproval</t>
   </si>
   <si>
     <t xml:space="preserve">Superintendent of Approval</t>
   </si>
   <si>
-    <t xml:space="preserve">vaibhav/APPVL-Superintendent-01</t>
+    <t xml:space="preserve">SUPAPP1/ADM_Superintendent of Approval_2</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -407,6 +407,11 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -454,7 +459,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,6 +477,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,18 +504,18 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,6 +534,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -542,6 +552,7 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -559,6 +570,7 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -576,6 +588,7 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -593,6 +606,7 @@
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -610,6 +624,7 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -627,6 +642,7 @@
       <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="F7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -644,6 +660,7 @@
       <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -658,6 +675,8 @@
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -672,6 +691,8 @@
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -686,6 +707,8 @@
       <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -700,6 +723,8 @@
       <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -714,6 +739,8 @@
       <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -731,6 +758,7 @@
       <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -748,6 +776,7 @@
       <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="F15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -765,6 +794,7 @@
       <c r="E16" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="F16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -782,6 +812,7 @@
       <c r="E17" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="F17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
@@ -882,6 +913,7 @@
       <c r="D23" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
@@ -942,46 +974,46 @@
         <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>92</v>
@@ -1036,8 +1068,8 @@
       <c r="A34" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>82</v>
+      <c r="B34" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>104</v>
@@ -1051,7 +1083,7 @@
         <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>107</v>
@@ -1063,7 +1095,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1084,12 +1116,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1110,12 +1142,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-6084] UI : Added the workflow for the creation of Agreement in LAMS module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t xml:space="preserve">SUPAPP1/ADM_Superintendent of Approval_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veeraswamy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Veeraswamy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissionerLAMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -407,11 +419,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -459,7 +466,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -477,10 +484,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,20 +505,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,7 +1071,7 @@
       <c r="A34" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1091,6 +1094,35 @@
       <c r="D35" s="1" t="s">
         <v>108</v>
       </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1115,9 +1147,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1141,9 +1170,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-5999] Modified the DEE name in excel
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -159,7 +159,7 @@
     <t xml:space="preserve">Deputy Executive Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_4</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to DEE</t>
@@ -507,18 +507,18 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1127,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1147,10 +1147,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1170,10 +1173,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[PHOENIX-5849] UI : Fixed UI Automation for Finance Module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">Commissioner</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
+    <t xml:space="preserve">CommissionerTest ~ ADN Comm</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to commissioner</t>
@@ -96,7 +96,7 @@
     <t xml:space="preserve">commissioner1</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+    <t xml:space="preserve">CommissionerTest/ADN Comm</t>
   </si>
   <si>
     <t xml:space="preserve">engineer1</t>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
   </si>
   <si>
-    <t xml:space="preserve">accountOfficer1</t>
+    <t xml:space="preserve">assExaminerOfAccounts</t>
   </si>
   <si>
     <t xml:space="preserve">ACCOUNTS</t>
@@ -129,28 +129,34 @@
     <t xml:space="preserve">Assistant Examiner of Accounts</t>
   </si>
   <si>
-    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer2</t>
+    <t xml:space="preserve">AssExaminerTest ~ ACC AEOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Assistant Examiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinerOfAccounts</t>
   </si>
   <si>
     <t xml:space="preserve">Examiner of Accounts</t>
   </si>
   <si>
-    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
+    <t xml:space="preserve">ExaminerTest ~ ACC EOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Examiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assExaminerOfAccounts1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssExaminerTest/ACC AEOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examinerOfAccounts1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExaminerTest/ACC EOA</t>
   </si>
   <si>
     <t xml:space="preserve">deputyExecutiveEngineer</t>
@@ -367,8 +373,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -466,12 +473,16 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -505,23 +516,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +550,7 @@
       </c>
       <c r="F1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -557,7 +568,7 @@
       </c>
       <c r="F2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -575,7 +586,7 @@
       </c>
       <c r="F3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -593,7 +604,7 @@
       </c>
       <c r="F4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -611,7 +622,7 @@
       </c>
       <c r="F5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -629,7 +640,7 @@
       </c>
       <c r="F6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -647,7 +658,7 @@
       </c>
       <c r="F7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -665,7 +676,7 @@
       </c>
       <c r="F8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -675,472 +686,464 @@
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="0"/>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="0"/>
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="0"/>
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="0"/>
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="F12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>31</v>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>66</v>
+      <c r="C21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="0"/>
       <c r="F22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>71</v>
+    <row r="23" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="0"/>
+        <v>77</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>74</v>
+    <row r="24" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="F24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="F25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1166,7 +1169,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1192,7 +1195,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[PHOENIX-6061] UI : Fixed automation for Grievances
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -198,10 +198,7 @@
     <t xml:space="preserve">LightingSuperintendent</t>
   </si>
   <si>
-    <t xml:space="preserve">Lighting Superintendent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAGADEESH MADARAPU</t>
+    <t xml:space="preserve">U.Srinivasulu</t>
   </si>
   <si>
     <t xml:space="preserve">Sanctioned and shall grievance be processed</t>
@@ -377,7 +374,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -404,6 +401,11 @@
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -468,12 +470,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -486,7 +488,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,7 +500,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,17 +525,17 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -806,49 +812,49 @@
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -858,7 +864,7 @@
     </row>
     <row r="19" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
@@ -866,7 +872,7 @@
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -876,7 +882,7 @@
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -884,8 +890,8 @@
       <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>68</v>
+      <c r="D20" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>48</v>
@@ -894,41 +900,41 @@
     </row>
     <row r="21" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E22" s="0"/>
       <c r="F22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>76</v>
+      <c r="A23" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -937,7 +943,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -946,7 +952,7 @@
     </row>
     <row r="24" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -955,16 +961,16 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -973,7 +979,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -982,142 +988,142 @@
     </row>
     <row r="26" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="F26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="F31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
@@ -1126,13 +1132,13 @@
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
@@ -1141,7 +1147,7 @@
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="0"/>
     </row>
@@ -1169,7 +1175,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1195,7 +1201,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>